<commit_message>
small changes in code and test scenarios
</commit_message>
<xml_diff>
--- a/Testovací scénáře.xlsx
+++ b/Testovací scénáře.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sochor\Desktop\ENGETO projekty\Task-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6D62B4-3D62-45CA-B2E5-62021CFA4022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8F109E-5B62-42DC-BBC2-8F013584EB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="584" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hlavni_menu" sheetId="1" r:id="rId1"/>
+    <sheet name="pridat_ukol" sheetId="2" r:id="rId2"/>
+    <sheet name="zobrazit_ukoly" sheetId="3" r:id="rId3"/>
+    <sheet name="odstranit_ukol" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
   <si>
     <t>TC01: Zobrazení hlavního menu</t>
   </si>
@@ -83,6 +86,80 @@
   </si>
   <si>
     <t>TC03:</t>
+  </si>
+  <si>
+    <t>TC01: Přidání nového úkolu</t>
+  </si>
+  <si>
+    <t>Přidání nového úkolu a jeho popisu do celkového seznamu úkolů</t>
+  </si>
+  <si>
+    <t>Program je spuštěný a nabízí uživateli možnost přidat nový úkol</t>
+  </si>
+  <si>
+    <t>1. Spustit program v editoru nebo přes CMD
+2. Vybrat možnost přidání nového úkolu
+3. Vyplnění názvu úkolu
+4. Vyplnění popisu úkolu</t>
+  </si>
+  <si>
+    <t>Program nabídne uživateli zadat název a popis úkolu a přidá zadaný úkol s popisem do seznamu úkolů</t>
+  </si>
+  <si>
+    <t>Program správně vybídl uživatele k vyplnění názvu úkolu a popisu a přidal úkol do seznamu</t>
+  </si>
+  <si>
+    <t>TC01: Odstranění existujícího úkolu</t>
+  </si>
+  <si>
+    <t>TC02: Odstranění neexistujícího úkolu</t>
+  </si>
+  <si>
+    <t>TC01: Přidání několika úkolů</t>
+  </si>
+  <si>
+    <t>Přidání několika úkolů do seznamu</t>
+  </si>
+  <si>
+    <t>1. Spustit program v editoru nebo přes CMD
+2. Vybrat možnost přidání nového úkolu
+3. Vyplnění názvu úkolu
+4. Vyplnění popisu úkolu
+5. Zopakovat přidání úkolu ještě minimálně jednou</t>
+  </si>
+  <si>
+    <t>Program nabídne uživateli zadat název a popis úkolu a přidá všechny úkoly s popisem do seznamu úkolů</t>
+  </si>
+  <si>
+    <t>Program pokaždé správně vybídl uživatele k vyplnění názvu úkolu a popisu a přidal každý jednotlivý úkol do seznamu</t>
+  </si>
+  <si>
+    <t>Důležité pro zjištění, že se funkce nerozbije při zadání více než jen jednoho úkolu</t>
+  </si>
+  <si>
+    <t>TC01: Zobrazení seznamu úkolů, kde je alespoň 1 úkol</t>
+  </si>
+  <si>
+    <t>TC01: Zobrazení seznamu úkolů, kde není žádný úkol</t>
+  </si>
+  <si>
+    <t>Uživatel odstraní úkol, který je uložený v seznamu úkolů</t>
+  </si>
+  <si>
+    <t>Uživatel zobrazí seznam úkolů, ve kterém je uložený alespoň 1 úkol</t>
+  </si>
+  <si>
+    <t>V seznamu úkolů je uložený alespoň 1 úkol</t>
+  </si>
+  <si>
+    <t>1. Uživatel uloží úkol do seznamu (prerekvizita)
+2. Uživatel vybere možnost zobrazit úkoly</t>
+  </si>
+  <si>
+    <t>Program zobrazí seznam úkolů</t>
+  </si>
+  <si>
+    <t>Program zobrazil seznam uložených úkolů</t>
   </si>
 </sst>
 </file>
@@ -430,9 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -554,7 +629,7 @@
       <c r="B17" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -562,4 +637,357 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0187178-B5BE-4A54-A57D-9F7C2D8AF400}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E9D66A-242C-47D9-8263-D8561366B7F7}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127852D9-1A62-48A1-8767-B00EDCAF822A}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added and cleaned up some code + added more test cases.
</commit_message>
<xml_diff>
--- a/Testovací scénáře.xlsx
+++ b/Testovací scénáře.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sochor\Desktop\ENGETO projekty\Task-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8F109E-5B62-42DC-BBC2-8F013584EB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88C3DB7-24F4-43E6-BB06-A2A13638081F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="584" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hlavni_menu" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
   <si>
     <t>TC01: Zobrazení hlavního menu</t>
   </si>
@@ -140,9 +140,6 @@
     <t>TC01: Zobrazení seznamu úkolů, kde je alespoň 1 úkol</t>
   </si>
   <si>
-    <t>TC01: Zobrazení seznamu úkolů, kde není žádný úkol</t>
-  </si>
-  <si>
     <t>Uživatel odstraní úkol, který je uložený v seznamu úkolů</t>
   </si>
   <si>
@@ -160,6 +157,30 @@
   </si>
   <si>
     <t>Program zobrazil seznam uložených úkolů</t>
+  </si>
+  <si>
+    <t>TC03: Přidání úkolu bez názvu</t>
+  </si>
+  <si>
+    <t>Přidání úkolu s nevyplněným názvem a popisem</t>
+  </si>
+  <si>
+    <t>1. Spustit program
+2. Vybrat možnost přidání nového úkolu
+3. Nevyplnit název a pokračovat dále
+4. Nevyplnit popis a uložit úkol bez názvu a popisu</t>
+  </si>
+  <si>
+    <t>Důležité pro zjištění, že uživatel nemůže vložit do seznamu prázdný úkol. Jedná se o negativní testovací případ, který správně nemá projít.</t>
+  </si>
+  <si>
+    <t>Program pokaždé správně vybídl uživatele k vyplnění názvu úkolu a popisu.</t>
+  </si>
+  <si>
+    <t>Program uživatele upozorní u obou kroků, že musí zadat název i popis. Uživatel nemůže nechat název a popis úkolu prázdný.</t>
+  </si>
+  <si>
+    <t>TC02: Zobrazení prázdného seznamu úkolů</t>
   </si>
 </sst>
 </file>
@@ -507,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -641,7 +662,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0187178-B5BE-4A54-A57D-9F7C2D8AF400}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -772,6 +793,67 @@
         <v>32</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -781,9 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E9D66A-242C-47D9-8263-D8561366B7F7}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -798,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -806,7 +886,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -814,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +902,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -830,7 +910,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -847,7 +927,7 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,9 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127852D9-1A62-48A1-8767-B00EDCAF822A}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -914,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test + added some TCs
</commit_message>
<xml_diff>
--- a/Testovací scénáře.xlsx
+++ b/Testovací scénáře.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sochor\Desktop\ENGETO projekty\Task-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88C3DB7-24F4-43E6-BB06-A2A13638081F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A07CD6-DE1D-41A3-894B-B8C0A901CB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="584" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hlavni_menu" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
   <si>
     <t>TC01: Zobrazení hlavního menu</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>TC02: Odstranění neexistujícího úkolu</t>
-  </si>
-  <si>
-    <t>TC01: Přidání několika úkolů</t>
   </si>
   <si>
     <t>Přidání několika úkolů do seznamu</t>
@@ -181,6 +178,34 @@
   </si>
   <si>
     <t>TC02: Zobrazení prázdného seznamu úkolů</t>
+  </si>
+  <si>
+    <t>TC02: Přidání několika úkolů</t>
+  </si>
+  <si>
+    <t>TC03: Odstranění neexistujícího úkolu</t>
+  </si>
+  <si>
+    <t>Uživatel má uložený alespoň 1 úkol v seznamu úkolů</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Uživatel vybere možnost Odstranit úkol
+2. Uživatel vybere z nabízených úkolů ten, který chce odstranit
+</t>
+  </si>
+  <si>
+    <t>Program odstraní úkol ze seznamu a nadále ho při zobrazení úkolů již nezobrazuje</t>
+  </si>
+  <si>
+    <t>Program úkol úspěšně odstranil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Uživatel vybere možnost Odstranit úkol
+2. Uživatel vybere k odstranění číslo úkolu, které se v seznamů úkolů nenachází (např. větší číslo, než kolik je celkový počet úkolů v seznamu)
+</t>
+  </si>
+  <si>
+    <t>Program nabídne uživateli hlášku o tom, že daný úkol neexistuje</t>
   </si>
 </sst>
 </file>
@@ -528,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -668,7 +693,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
     <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -734,7 +759,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -758,7 +783,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -766,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -774,7 +799,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,12 +815,12 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -827,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -835,7 +860,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +876,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +894,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -878,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -886,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -894,7 +919,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +927,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -910,7 +935,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,7 +952,7 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -972,9 +997,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127852D9-1A62-48A1-8767-B00EDCAF822A}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -982,72 +1009,100 @@
     <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,6 +1117,46 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>